<commit_message>
Fix subcategory editing and rename logic with data preservation
</commit_message>
<xml_diff>
--- a/outputs/gantt_FINAL_VERIFICADO_314.xlsx
+++ b/outputs/gantt_FINAL_VERIFICADO_314.xlsx
@@ -8,19 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fd171dda8de17894/Desktop/cerebro-patio/Cerebro/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_8A1B9FA788E048D30200D077923BBB562BBB017C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC0D2D08-6666-4F79-9F9D-44DFCD772FEF}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_8A1B9FA788E048D30200D077923BBB562BBB017C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CA44AEA-FF18-468F-8A2E-C3AA95350448}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="2500" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Gantt L-V" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Gantt L-V'!$E$7:$U$42</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Gantt L-V'!$E$4:$U$42</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -629,14 +624,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC96032F-A8E9-4862-9CBC-6428D2D163BF}">
   <dimension ref="D2:U21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -715,7 +707,7 @@
         <v>domingo</v>
       </c>
     </row>
-    <row r="4" spans="4:21" s="1" customFormat="1" ht="53.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="4:21" s="1" customFormat="1" ht="52.9" x14ac:dyDescent="0.45">
       <c r="E4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1169,10 +1161,9 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:E1048576">
+  <conditionalFormatting sqref="E1:E5 E19:E1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125978" footer="0.31496062992125978"/>
-  <pageSetup scale="71" orientation="landscape"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>